<commit_message>
Added intensity and bar graphs
</commit_message>
<xml_diff>
--- a/data/Energy_Data_for_Net_Zero_Study.xlsx
+++ b/data/Energy_Data_for_Net_Zero_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8610e9849f4c2023/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\Documents\R\RockCenterEnergyAnalysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{D9D85C87-89AB-4512-89A2-91CBF3ACF754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F573B7-DAA3-4021-8B90-322D487D9325}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB04008-04C6-4E4A-93AB-5DCED862B65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8610" yWindow="3075" windowWidth="9638" windowHeight="8003" xr2:uid="{846456E4-5EAC-4733-BC23-256F5A889430}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{846456E4-5EAC-4733-BC23-256F5A889430}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>10 rock</t>
   </si>
@@ -469,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3857281A-FA2A-4F61-ABF0-4FD295FE7573}">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -964,6 +964,102 @@
         <v>1.0861290322580646</v>
       </c>
     </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>487541</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>808600</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>2911536</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>1217115</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>111101</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>472505</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>147585</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>449291</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>482357</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>482358</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>964715</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>